<commit_message>
lior - post meeting updates
</commit_message>
<xml_diff>
--- a/acceptance_tests_v2.xlsx
+++ b/acceptance_tests_v2.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DD1BA7-1261-4ED0-80FF-B447616CCD53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9780"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>#</t>
   </si>
@@ -43,24 +44,10 @@
     <t>operation, wrong id</t>
   </si>
   <si>
-    <t xml:space="preserve">1.the operation will stop and
-the car wont get refuled
-2.the system will print:
-"no such client exists, please
-register to the system via 
-marketing representative"
-</t>
-  </si>
-  <si>
     <t>the NFC id is not recognizable</t>
   </si>
   <si>
     <t>operation, no NFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.the operation will stop and
-the car wont get refuled
-</t>
   </si>
   <si>
     <t>1. the car does not have NFC 
@@ -75,234 +62,323 @@
 successful</t>
   </si>
   <si>
-    <t>client fills a purchase request 
-in the correct way 
-and the system create such order</t>
-  </si>
-  <si>
-    <t>1.system prints: "amount cant be
-negative please fill again"
-2.system clears the amount field</t>
-  </si>
-  <si>
     <t>client fills a negative amount of 
 fuel</t>
   </si>
   <si>
-    <t>1.system prints: "amount cant be
-with charcters please fill again"
-2.system clears the amount field</t>
-  </si>
-  <si>
-    <t>home fuel purchase 
-wrong shipment</t>
-  </si>
-  <si>
-    <t>1.system prints: "please select
-a shipment method"
-2.system highlights the combo box of
-shipment method</t>
-  </si>
-  <si>
-    <t>client does not choose any
-shipment method</t>
-  </si>
-  <si>
-    <t>1.the pumps works and the
+    <t>the NFC id is correct</t>
+  </si>
+  <si>
+    <t>fueling operation completed succssefuly</t>
+  </si>
+  <si>
+    <t>operation, no
+fuel</t>
+  </si>
+  <si>
+    <t>operation, not enough fuel</t>
+  </si>
+  <si>
+    <t>operation stops becuase 
+there is no fuel 
+in the pump</t>
+  </si>
+  <si>
+    <t>fueling operation has been done but not in the required capacity</t>
+  </si>
+  <si>
+    <t>1. the pump works and the
 car gets fuel
-2.the system shows the client
+2. the system shows the client
 his rate by his current business
 conditions
-3.system sends the payment to an external system
-4.the system recalculate current
-fuel capacity in storage</t>
-  </si>
-  <si>
-    <t>the NFC id is correct</t>
-  </si>
-  <si>
-    <t>1.the NFC id= 223344 belong to a client
+3. the system sends the payment to an external system
+4. the system recalculates current
+fuel capacity in storage
+5. the system saves the purchase</t>
+  </si>
+  <si>
+    <t>1. the NFC id = 223344 belongs to a client
 that is registered to the system
 2. there is enough fuel in the required 
 fuel type in the pump</t>
   </si>
   <si>
-    <t xml:space="preserve">1. the NFC id=111111 does not belong
-to any client in the DB
+    <t>1. the system shows "invalid NFC" on the pump's screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. the NFC id = 111111 does not belong
+to any client in the database
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1.the operation will stop and
-the car wont get refuled
-2.system will print "there is no fuel
-in this pump, please change to other pump"
-</t>
-  </si>
-  <si>
-    <t>operation , fuel is under the threshold</t>
-  </si>
-  <si>
-    <t>1.the pumps works and the
+    <t>1. the operation will stop and
+the car won't get refueled</t>
+  </si>
+  <si>
+    <t>1. the operation will stop and
+the car won't get refueled
+2. the system will show "not enough fuel, change pump" on the pump's screen</t>
+  </si>
+  <si>
+    <t>1. the NFC id = 223344 belongs to a client
+that is registered to the system
+2. there is no fuel in the required 
+fuel type in the pump</t>
+  </si>
+  <si>
+    <t>operation, fuel is under the threshold</t>
+  </si>
+  <si>
+    <t>1. the pump works and the
 car gets fuel
-2.the system shows the client
+2. the system shows the client
 his rate by his current business
 conditions
-3.system sends the payment to an external system
-4.the system recalculate current
+3. the system sends the payment to an external system
+4. the system recalculates current
 fuel capacity in storage
-5. system alerts the fuel station manager
-6. system creates an order</t>
-  </si>
-  <si>
-    <t>1.the NFC id= 223344 belong to a client
+5. the system saves the purchase
+6. system alerts the fuel station manager
+7. system creates an order</t>
+  </si>
+  <si>
+    <t>1. the NFC id = 223344 belongs to a client
 that is registered to the system
 2. there is enough fuel in the required 
 fuel type in the pump
-3. the pump has higher fuel capacity than the threshold</t>
-  </si>
-  <si>
-    <t>fueling operation completed succssefuly</t>
-  </si>
-  <si>
-    <t>operation, no
-fuel</t>
-  </si>
-  <si>
-    <t>operation, not enough fuel</t>
-  </si>
-  <si>
-    <t>operation stops becuase 
-there is no fuel 
-in the pump</t>
-  </si>
-  <si>
-    <t>1.the pumps works and the
-car gets fuel until the pump is empty
-2.system prints "the pump is now empty"
-3.the system shows the client
+3. the pump has a higher fuel capacity than the threshold</t>
+  </si>
+  <si>
+    <t>1. the pump works and the
+car gets fuel
+2. the system shows "pump is now empty" on the pump's screen
+3. the system shows the client
 his rate by his current business
 conditions
-4.system sends the payment to an external system
-5.the system recalculate current
+4. the system sends the payment to an external system
+5. the system recalculates current
 fuel capacity in storage
-6. system creates an order</t>
-  </si>
-  <si>
-    <t>1.the NFC id= 223344 belong to a client
+6. the system saves the purchase
+7. system alerts the fuel station manager
+8. system creates an order</t>
+  </si>
+  <si>
+    <t>1. the NFC id = 223344 belongs to a client
 that is registered to the system
-2. there is not enough fuel in the required 
-capacity in the pump
-3. the pump has lower fuel capacity than the threshold</t>
-  </si>
-  <si>
-    <t>fueling operation has been done but not in the required capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. choose  the fuel pump
-2.put the pump handle to the chamber
-3. use an NFC sensor witch has the
+2. there is no fuel in the required 
+fuel type in the pump
+3. the pump has a lower fuel capacity than the threshold</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type from list
+3. sets field 'fuel amount' = 500
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>client fills 'fuel amount' = 0</t>
+  </si>
+  <si>
+    <t>1. client fills a purchase request 
+in the correct way 
+and the system create such order
+2. client fills 'fuel amount' below 600</t>
+  </si>
+  <si>
+    <t>1. client fills a purchase request 
+in the correct way 
+and the system create such order
+2. client fills 'fuel amount' between 600 and 800</t>
+  </si>
+  <si>
+    <t>1. client fills a purchase request 
+in the correct way 
+and the system create such order
+2. client fills 'fuel amount' above 800</t>
+  </si>
+  <si>
+    <t>1. client chooses the fuel pump
+2. put the pump handle to the chamber
+3. use an NFC sensor which has the
+following data:
+3.a. NFC id = 223344
+4. wait for pump to be ready
+5. start refueling</t>
+  </si>
+  <si>
+    <t>1. client chooses the fuel pump
+2. put the pump handle to the chamber
+3. use an NFC sensor which has the
+following data:
+3.a. NFC id = 111111</t>
+  </si>
+  <si>
+    <t>1. client chooses the fuel pump
+2. put the pump handle to the chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. client chooses the fuel pump
+2. put the pump handle to the chamber
+3. use an NFC sensor which has the
 following data:
 3.a. NFC id = 223344
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1. choose  the fuel pump
-2.put the pump handle to the chamber
-3. use an NFC sensor witch has the
+    <t>1. client chooses the fuel pump
+2. put the pump handle to the chamber
+3. use an NFC sensor which has the
 following data:
 3.a. NFC id = 223344
 4. wait for pump to be ready
-5. start fueling
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. choose  the fuel pump
-2.put the pump handle to the chamber
-3. use an NFC sensor witch has the
-following data:
-3.a. NFC id = 111111
-</t>
-  </si>
-  <si>
-    <t>1. choose  the fuel pump
-2.put the pump handle to the chamber</t>
-  </si>
-  <si>
-    <t>1. choose  the fuel pump
-2.put the pump handle to the chamber
-3. use an NFC sensor witch has the
-following data:
-3.a. NFC id = 223344
-4. wait for pump to be ready
-5. fuel the car until the fuel in the pump is lower than the "low threshold"</t>
-  </si>
-  <si>
-    <t>1.the NFC id= 223344 belong to a client
-that is registered to the system
-2.the NFC fuel type is 
-recognized in the system
-3. there is no fuel in the required
-fuel type in the pump</t>
-  </si>
-  <si>
-    <t>1. user is logged into the system
-2. there is enough fuel</t>
-  </si>
-  <si>
-    <t>1.system saves the purchase
-info after finishing refuling
-2.the system recalculate current 
-fuel capacity in storage
-3.system prints "purchase approved"
-4. system sends the payment order to an external system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. user is logged into the system
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home fuel purchase 
-wrong fuel amount- characters </t>
+5. refuel the car until the fuel in the pump is lower than the "low threshold"</t>
   </si>
   <si>
     <t>home fuel purchase 
-wrong fuel amount-
-negative 
-number</t>
-  </si>
-  <si>
-    <t>1. user choose "home fuel purchas"
-2.dont choose shipment method from 
-combo box
-3.set in field "fuel amount" = 500
-4.press button "Confrim Purchase"</t>
-  </si>
-  <si>
-    <t>1. user choose "home fuel purchas"
-2.choose shipment method from 
-combo box
-3.set in field "fuel amount" = aaa
-4.press button "Confrim Purchase"</t>
-  </si>
-  <si>
-    <t>1. user choose "home fuel purchas"
-2.choose shipment method from 
-combo box
-3.set in field "fuel amount" = -5
-4.press button "Confrim Purchase"</t>
-  </si>
-  <si>
-    <t>1. user choose "home fuel purchas"
-2.choose shipment method from 
-combo box
-3.set in field "fuel amount" = 500
-4.press button "Confrim Purchase"</t>
+successful - discount</t>
+  </si>
+  <si>
+    <t>home fuel purchase 
+successful - highest discount</t>
+  </si>
+  <si>
+    <t>1. the system saves the purchase
+2. the system sends the payment order to an external system</t>
+  </si>
+  <si>
+    <t>the client is logged into the system</t>
+  </si>
+  <si>
+    <t>client does not choose any
+shipment type</t>
+  </si>
+  <si>
+    <t>1. client fills a purchase request 
+in the correct way 
+and the system create such order
+2. client chooses 'regular order'</t>
+  </si>
+  <si>
+    <t>1. client fills a purchase request 
+in the correct way 
+and the system create such order
+2. client chooses 'urgent order'</t>
+  </si>
+  <si>
+    <t>home fuel purchase, 
+negative fuel amount</t>
+  </si>
+  <si>
+    <t>home fuel purchase, 
+zero fuel amount</t>
+  </si>
+  <si>
+    <t>home fuel purchase, 
+invalid fuel amount</t>
+  </si>
+  <si>
+    <t>home fuel purchase, no shipment type</t>
+  </si>
+  <si>
+    <t>home fuel purchase, regular shipment type</t>
+  </si>
+  <si>
+    <t>home fuel purchase, urgent shipment type</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type from list
+3. sets field 'fuel amount' = 700
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type from list
+3. sets field 'fuel amount' = 900
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>1. the system saves the purchase
+2. the system recalculates purchase fee
+(-4% of order price)
+3. the system sends the payment order to an external system</t>
+  </si>
+  <si>
+    <t>1. the system saves the purchase
+2. the system recalculates purchase fee
+(-3% of order price)
+3. the system sends the payment order to an external system</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type from list
+3. sets field 'fuel amount' = -5
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type from list
+3. sets field 'fuel amount' = 0
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>client does not fill any
+amount of fuel</t>
+  </si>
+  <si>
+    <t>home fuel purchase, 
+no fuel amount</t>
+  </si>
+  <si>
+    <t>the system prints "amount invalid"</t>
+  </si>
+  <si>
+    <t>the system prints "missing fields"</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type from list
+3. sets field 'fuel amount' = aaa
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type from list
+3. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. sets field 'fuel amount' = 500
+3. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>client fills non-digits in amount of 
+fuel</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type 'regular'
+3. fills 'fuel amount'
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>1. the client chooses "home fuel purchase"
+2. chooses shipment type 'urgent'
+3. fills 'fuel amount'
+4. press button "confrim purchase"</t>
+  </si>
+  <si>
+    <t>1. the system saves the purchase
+2. the system recalculates purchase fee
+(+2% of fuel price)
+3. the system sends the payment order to an external system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,16 +513,22 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1766894" cy="405432"/>
+    <xdr:ext cx="1587486" cy="405432"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4068536" y="231321"/>
-          <a:ext cx="1766894" cy="405432"/>
+          <a:off x="4174191" y="231321"/>
+          <a:ext cx="1587486" cy="405432"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -475,7 +557,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="2000"/>
-            <a:t>Fast Fuels tests</a:t>
+            <a:t>fast fuel tests</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -485,19 +567,25 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1802609" cy="405432"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3592286" y="8885464"/>
+          <a:off x="3989294" y="10880912"/>
           <a:ext cx="1802609" cy="405432"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -536,110 +624,98 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2446</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1852173</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>302559</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1890380</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1120753</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="תמונה 4" descr="https://media.discordapp.net/attachments/689045729414610980/693506719237668964/unknown.png?width=768&amp;height=369"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50171073-02DB-42FF-832B-57F0E9E5217B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="11107475" y="10021261"/>
-          <a:ext cx="11192231" cy="5409238"/>
+          <a:off x="11721353" y="806824"/>
+          <a:ext cx="4904762" cy="3171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2454088</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>549088</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>258295</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2022031</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>42144</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="תמונה 7" descr="https://media.discordapp.net/attachments/689045729414610980/693516645028593674/unknown.png?width=768&amp;height=346"/>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC163014-0735-41FB-BDC8-46B73D987FC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="10925735" y="1008529"/>
-          <a:ext cx="7261412" cy="3295090"/>
+          <a:off x="11710147" y="11441206"/>
+          <a:ext cx="5047619" cy="3504762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -648,7 +724,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -723,6 +799,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -758,6 +851,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -933,11 +1043,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,6 +1056,8 @@
     <col min="3" max="3" width="35.42578125" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" customWidth="1"/>
     <col min="5" max="6" width="37.5703125" customWidth="1"/>
+    <col min="13" max="13" width="38.42578125" customWidth="1"/>
+    <col min="14" max="33" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -977,16 +1089,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -997,16 +1109,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1014,42 +1126,42 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="153" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -1066,27 +1178,27 @@
         <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1110,44 +1222,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1155,19 +1267,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1175,23 +1287,143 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>9</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1201,7 +1433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1213,7 +1445,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>